<commit_message>
Board Version 1.0 Review 3
</commit_message>
<xml_diff>
--- a/Hardware/010_Implementation/BOM.xlsx
+++ b/Hardware/010_Implementation/BOM.xlsx
@@ -1215,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,10 +1945,10 @@
       <c r="E34" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">

</xml_diff>

<commit_message>
Added Control List to BOM Excel Table
</commit_message>
<xml_diff>
--- a/Hardware/010_Implementation/BOM.xlsx
+++ b/Hardware/010_Implementation/BOM.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Board" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="97">
   <si>
     <t>Id</t>
   </si>
@@ -823,7 +824,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -845,6 +846,15 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1215,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,4 +2055,545 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>9</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>11</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="10">
+        <v>150</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>12</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10">
+        <v>430</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>13</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10">
+        <v>500</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>14</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="10">
+        <v>100</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>15</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>16</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="10">
+        <v>62</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>17</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>18</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>19</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>20</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>21</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>22</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>23</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>24</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>25</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>26</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>27</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="10">
+        <v>744242220</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>28</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>29</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>30</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>31</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>32</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>33</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>34</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>35</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>36</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>37</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>38</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM with missing component and correct values
</commit_message>
<xml_diff>
--- a/Hardware/010_Implementation/BOM.xlsx
+++ b/Hardware/010_Implementation/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="100">
   <si>
     <t>Id</t>
   </si>
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>https://www.digikey.de/short/zv370m</t>
+  </si>
+  <si>
+    <t>C18,C17,C14,C13,C11,C10,C9,C8,C1</t>
+  </si>
+  <si>
+    <t>910k</t>
+  </si>
+  <si>
+    <t>3,3n</t>
   </si>
 </sst>
 </file>
@@ -2062,7 +2071,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G17" sqref="G17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2203,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>23</v>
@@ -2236,7 +2245,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="10">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>23</v>
@@ -2312,12 +2321,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>19</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>13</v>
@@ -2334,7 +2343,7 @@
         <v>40</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>38</v>

</xml_diff>